<commit_message>
subnets note intopacket tracer
</commit_message>
<xml_diff>
--- a/subnets_L2b_Tinklai.xlsx
+++ b/subnets_L2b_Tinklai.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rytis\Desktop\Tinklai_l2b\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765CD411-4683-4DD8-BD1D-DE2993406128}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC99325-4761-4B48-9F48-098CE9D45978}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>MTK2 16</t>
   </si>
@@ -106,6 +106,30 @@
   </si>
   <si>
     <t>172.18.5.209 - 172.18.5.222</t>
+  </si>
+  <si>
+    <t>Audit1</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Audit2</t>
+  </si>
+  <si>
+    <t>Multi</t>
+  </si>
+  <si>
+    <t>Diz</t>
+  </si>
+  <si>
+    <t>Egz</t>
+  </si>
+  <si>
+    <t>Dest, Elek</t>
+  </si>
+  <si>
+    <t>Ism</t>
   </si>
 </sst>
 </file>
@@ -438,15 +462,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C5:H15"/>
+  <dimension ref="B5:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="14.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.77734375" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.88671875" style="1"/>
     <col min="5" max="5" width="19.6640625" style="1" customWidth="1"/>
@@ -456,7 +481,10 @@
     <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B5" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
@@ -470,7 +498,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
@@ -484,7 +515,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B7" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
@@ -498,7 +532,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="C9" s="1" t="s">
         <v>0</v>
       </c>
@@ -512,7 +549,10 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="C10" s="1" t="s">
         <v>1</v>
       </c>
@@ -526,7 +566,10 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B12" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="C12" s="1" t="s">
         <v>5</v>
       </c>
@@ -540,7 +583,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B14" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="C14" s="1" t="s">
         <v>6</v>
       </c>
@@ -554,7 +600,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B15" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="C15" s="1" t="s">
         <v>7</v>
       </c>

</xml_diff>